<commit_message>
CN Format First Commit...
</commit_message>
<xml_diff>
--- a/Courier/Tables.xlsx
+++ b/Courier/Tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21CAAC2-6231-44A6-9A11-2C0A74606E79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2BEB1D-647B-4666-BC21-10AFAB1E4219}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
   <si>
     <t>ACK_NAME</t>
   </si>
@@ -291,6 +291,45 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>cn_invoice</t>
+  </si>
+  <si>
+    <t>cn_invoice_no</t>
+  </si>
+  <si>
+    <t>cn_invoice_date</t>
+  </si>
+  <si>
+    <t>cn_invoice_taxable</t>
+  </si>
+  <si>
+    <t>cn_invoice_tax</t>
+  </si>
+  <si>
+    <t>cn_invoice_total</t>
+  </si>
+  <si>
+    <t>cn_invoice_gstin</t>
+  </si>
+  <si>
+    <t>cn_invoice_weight</t>
+  </si>
+  <si>
+    <t>cn_invoice_quantity</t>
+  </si>
+  <si>
+    <t>cn_invoice_mop</t>
+  </si>
+  <si>
+    <t>cn_vehicle</t>
+  </si>
+  <si>
+    <t>cn_vehicle_no.</t>
+  </si>
+  <si>
+    <t>cn_vehicle_type</t>
   </si>
 </sst>
 </file>
@@ -1073,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,15 +1625,12 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="5" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -1613,44 +1649,165 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A63:E63"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A56:E56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>